<commit_message>
Made a start on implementing GUI Manager Module.vi
</commit_message>
<xml_diff>
--- a/src/Design Documents/Design Spreadsheet.xlsx
+++ b/src/Design Documents/Design Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7FCCDE-7269-4E46-BFBA-5F7FB1172DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12676FF-56E3-4809-9025-27C2AB5688F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Spreadsheet" sheetId="1" r:id="rId1"/>
@@ -522,16 +522,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>370800</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1342350</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>114075</xdr:rowOff>
+      <xdr:rowOff>133125</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -546,8 +546,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5876925" y="4686300"/>
-          <a:ext cx="5400000" cy="1961925"/>
+          <a:off x="12372975" y="4705350"/>
+          <a:ext cx="6733500" cy="1961925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -601,16 +601,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1380450</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6714450</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>104550</xdr:rowOff>
+      <xdr:rowOff>133125</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -625,7 +625,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="123825" y="4676775"/>
+          <a:off x="6838950" y="4705350"/>
           <a:ext cx="5400000" cy="1961925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -696,6 +696,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1096290</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA3CCA1-0262-80E3-6E42-239278D59BE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="4724400"/>
+          <a:ext cx="6554115" cy="1371791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -966,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Progress towards implementing "Init Tickboxes.vi"
</commit_message>
<xml_diff>
--- a/src/Design Documents/Design Spreadsheet.xlsx
+++ b/src/Design Documents/Design Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12676FF-56E3-4809-9025-27C2AB5688F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA252BE3-9E25-4397-8744-2BFB9C505795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,7 +682,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>2. The User VI can't be inside a virtual folder when it's not open in a project, and it's now owned by a lvlib or lvclass</a:t>
+            <a:t>2. The User VI can't be inside a virtual folder when it's not open in a project, and it's not owned by a lvlib or lvclass</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented "Init Tickboxes.vi". Successfully tested initial state 0. The other initial states still need to be tested.
</commit_message>
<xml_diff>
--- a/src/Design Documents/Design Spreadsheet.xlsx
+++ b/src/Design Documents/Design Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA252BE3-9E25-4397-8744-2BFB9C505795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD47C135-D62B-422E-BE2E-E7FAB26BEF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="51">
   <si>
     <t>Design Spreadsheet</t>
   </si>
@@ -201,6 +201,24 @@
   </si>
   <si>
     <t>Impossible (3)</t>
+  </si>
+  <si>
+    <t>Multiple projects open. The VI is owned, but isn't in a virtual folder.</t>
+  </si>
+  <si>
+    <t>Multiple projects open. The VI is owned, and is in a virtual folder.</t>
+  </si>
+  <si>
+    <t>A single project open. The User VI is not owned, and is not inside a virtual folder.</t>
+  </si>
+  <si>
+    <t>A single project open. The User VI is not owned, but is inside a virtual folder.</t>
+  </si>
+  <si>
+    <t>A single project open. The User VI is owned, but is not inside a virtual folder.</t>
+  </si>
+  <si>
+    <t>A single project open. The User VI is owned, and is inside a virtual folder.</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,6 +1429,9 @@
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="F13" s="19" t="s">
         <v>14</v>
       </c>
@@ -1447,6 +1468,9 @@
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F14" s="19" t="s">
         <v>14</v>
       </c>
@@ -1483,6 +1507,9 @@
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F15" s="19" t="s">
         <v>14</v>
       </c>
@@ -1519,6 +1546,9 @@
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E16" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F16" s="19" t="s">
         <v>14</v>
       </c>
@@ -1555,6 +1585,9 @@
       <c r="D17" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F17" s="19" t="s">
         <v>14</v>
       </c>
@@ -1590,6 +1623,9 @@
       </c>
       <c r="D18" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
1. Created the "Testing Record" worksheet in the spreadsheet: Design Documents/Design Spreadsheet.xlsx 2. Created test cases for each of the 10 possible initial states inside the Test Cases folder. Manually ran through these tests and recorded the results in the Testing Record worksheet.
</commit_message>
<xml_diff>
--- a/src/Design Documents/Design Spreadsheet.xlsx
+++ b/src/Design Documents/Design Spreadsheet.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD47C135-D62B-422E-BE2E-E7FAB26BEF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD3CDBF-A525-48AF-ABEA-C10C229B0F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Spreadsheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing Record" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="63">
   <si>
     <t>Design Spreadsheet</t>
   </si>
@@ -73,9 +74,6 @@
     <t>Impossible (1)</t>
   </si>
   <si>
-    <t>Corresponds to when the User VI is opened on its own. Its not part of a library, class, or project.</t>
-  </si>
-  <si>
     <t>Initial State Notes</t>
   </si>
   <si>
@@ -124,20 +122,7 @@
     <t>Impossible (2)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Corresponds to when the User VI is owned, but a project isn't open. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TO TEST</t>
-    </r>
+    <t>Corresponds to when the User VI is owned, but a project isn't open.</t>
   </si>
   <si>
     <r>
@@ -175,40 +160,15 @@
     <t>IS15</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Corresponds to when the User VI is owned and inside a Virtual Folder, but a project isn't open. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TO TEST</t>
-    </r>
-  </si>
-  <si>
     <t>"Add to Owner?" checkbox is enabled, but unticked. The "Add to Virtual Folder?" checkbox being ticked implies that the Add to Owner is also ticked.</t>
   </si>
   <si>
-    <t>Multiple projects open. The VI is likely inside one of the open projects, but we don't know which one.</t>
-  </si>
-  <si>
     <t>Enable the "Add to Project?" checkbox. Give the user the option to select which project to add to using the drop-down list. But don't tick it by default, because the user must choose which project. The app may assume wrong and insert into the wrong project, which will cause pain.</t>
   </si>
   <si>
     <t>Impossible (3)</t>
   </si>
   <si>
-    <t>Multiple projects open. The VI is owned, but isn't in a virtual folder.</t>
-  </si>
-  <si>
-    <t>Multiple projects open. The VI is owned, and is in a virtual folder.</t>
-  </si>
-  <si>
     <t>A single project open. The User VI is not owned, and is not inside a virtual folder.</t>
   </si>
   <si>
@@ -219,13 +179,65 @@
   </si>
   <si>
     <t>A single project open. The User VI is owned, and is inside a virtual folder.</t>
+  </si>
+  <si>
+    <t>Testing Record</t>
+  </si>
+  <si>
+    <t>LabVIEW 2022</t>
+  </si>
+  <si>
+    <t>Initial Situation</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>LabVIEW 2016</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Not Tested</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Corresponds to when the User VI is opened on its own. It's not part of a library, class, or project.</t>
+  </si>
+  <si>
+    <t>Tested with lvlib and lvclass owner. Passed both.</t>
+  </si>
+  <si>
+    <t>Corresponds to when the User VI is owned and inside a Virtual Folder, but a project isn't open.</t>
+  </si>
+  <si>
+    <t>Multiple projects open. The User VI is likely inside one of the open projects, but we don't know which one.</t>
+  </si>
+  <si>
+    <t>Multiple projects open. The User VI is owned, but isn't in a virtual folder.</t>
+  </si>
+  <si>
+    <t>Multiple projects open. The User VI is owned, and is in a virtual folder.</t>
+  </si>
+  <si>
+    <t>The Initial State configuration passed. Unable to insert into the virtual folder.</t>
+  </si>
+  <si>
+    <t>Initial Configuration
+Passed?</t>
+  </si>
+  <si>
+    <t>After-Launch Behaviour Passed?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,14 +271,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -293,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -335,6 +339,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -412,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -439,31 +463,31 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -475,18 +499,87 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -521,6 +614,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF5050"/>
       <color rgb="FF7DC8FF"/>
       <color rgb="FFFF7D7D"/>
     </mruColors>
@@ -1028,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1139,10 +1233,10 @@
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1186,7 +1280,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>13</v>
@@ -1207,10 +1301,10 @@
         <v>13</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1227,7 +1321,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>13</v>
@@ -1248,10 +1342,10 @@
         <v>13</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1268,7 +1362,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>13</v>
@@ -1289,7 +1383,7 @@
         <v>13</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M9" s="23"/>
     </row>
@@ -1307,7 +1401,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>13</v>
@@ -1328,10 +1422,10 @@
         <v>14</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1348,7 +1442,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>14</v>
@@ -1369,10 +1463,10 @@
         <v>13</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1389,7 +1483,7 @@
         <v>14</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>13</v>
@@ -1410,10 +1504,10 @@
         <v>13</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1430,7 +1524,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>14</v>
@@ -1451,7 +1545,7 @@
         <v>13</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M13" s="23"/>
     </row>
@@ -1469,7 +1563,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>14</v>
@@ -1490,7 +1584,7 @@
         <v>14</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M14" s="23"/>
     </row>
@@ -1508,7 +1602,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>14</v>
@@ -1529,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M15" s="23"/>
     </row>
@@ -1547,7 +1641,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>14</v>
@@ -1568,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="L16" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M16" s="23"/>
     </row>
@@ -1586,7 +1680,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>14</v>
@@ -1607,7 +1701,7 @@
         <v>13</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M17" s="23"/>
     </row>
@@ -1625,7 +1719,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>14</v>
@@ -1646,7 +1740,7 @@
         <v>14</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M18" s="23"/>
     </row>
@@ -1685,10 +1779,10 @@
         <v>13</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M19" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1726,10 +1820,10 @@
         <v>13</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1767,10 +1861,10 @@
         <v>13</v>
       </c>
       <c r="L21" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1808,10 +1902,10 @@
         <v>13</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1835,4 +1929,297 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF71B33-42AD-4C32-A9F4-2F19848A426B}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="34"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="34"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:C13 E4:F13">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B4:C13 E4:F13" xr:uid="{FB37DCCE-CA2A-4DD7-B48E-169B1B1B1FCF}">
+      <formula1>"Not Tested, Failed, Passed"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Built a new version of the LLB (1.3.0.4). Tested this version. Test results recorded in the "Testing Record" worksheet of Design Spreadsheet.xlsx
</commit_message>
<xml_diff>
--- a/src/Design Documents/Design Spreadsheet.xlsx
+++ b/src/Design Documents/Design Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD42F262-D7B3-453D-8E83-DCF9FE9EA06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C708B880-1400-45E4-860E-E1D8519C1391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Spreadsheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="80">
   <si>
     <t>Design Spreadsheet</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Multiple projects open. The User VI is owned, and is in a virtual folder.</t>
-  </si>
-  <si>
-    <t>The Initial State configuration passed. Unable to insert into the virtual folder.</t>
   </si>
   <si>
     <t>Initial Configuration
@@ -276,6 +273,20 @@
   </si>
   <si>
     <t>Checkbox Ticking/Unticking Behaviour Passed?</t>
+  </si>
+  <si>
+    <t>The Initial State configuration passed. Unable to insert into the virtual folder. The VI or CTL is inserted into the project, but not into the virtual folder.</t>
+  </si>
+  <si>
+    <t>Test Date: 12 Dec 2022
+LLB Version: 1.3.0.4</t>
+  </si>
+  <si>
+    <t>Error 56002 occurs when both ATP and ATO checkboxes are ticked. But the VI or CTL is correctl inserted into the lvlib owner.
+The error is completely repeatable. The same error occurs when VIs or CTLs are created. The same error occurs when the User VI is owned by lvlib or by lvclass.</t>
+  </si>
+  <si>
+    <t>Error 56002 occurs here too, just like in IS10. The VI or CTL is correctly inserted into the virtual folder.</t>
   </si>
 </sst>
 </file>
@@ -512,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -652,6 +663,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1200,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="F12" workbookViewId="0">
+    <sheetView topLeftCell="F14" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -1322,7 +1339,7 @@
       </c>
       <c r="M5" s="27"/>
       <c r="N5" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1394,7 +1411,7 @@
         <v>13</v>
       </c>
       <c r="N7" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1411,34 +1428,34 @@
         <v>14</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -1480,7 +1497,7 @@
         <v>13</v>
       </c>
       <c r="N9" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -1524,7 +1541,7 @@
         <v>14</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="75" x14ac:dyDescent="0.25">
@@ -1568,7 +1585,7 @@
         <v>13</v>
       </c>
       <c r="N11" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1585,34 +1602,34 @@
         <v>14</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -1654,7 +1671,7 @@
         <v>13</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="105" x14ac:dyDescent="0.25">
@@ -1696,7 +1713,7 @@
         <v>14</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1738,7 +1755,7 @@
         <v>13</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="105" x14ac:dyDescent="0.25">
@@ -1780,7 +1797,7 @@
         <v>14</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
@@ -1822,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="N17" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -1864,7 +1881,7 @@
         <v>14</v>
       </c>
       <c r="N18" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1881,34 +1898,34 @@
         <v>13</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G19" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N19" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N19" s="37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1925,34 +1942,34 @@
         <v>14</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N20" s="37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1969,34 +1986,34 @@
         <v>13</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G21" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N21" s="37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -2013,34 +2030,34 @@
         <v>14</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G22" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N22" s="37" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2069,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF71B33-42AD-4C32-A9F4-2F19848A426B}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,91 +2119,83 @@
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:15" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-    </row>
-    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="19" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+    </row>
+    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>51</v>
-      </c>
+      <c r="E5" s="16"/>
       <c r="F5" s="13" t="s">
         <v>48</v>
       </c>
@@ -2200,13 +2209,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>47</v>
@@ -2227,18 +2236,20 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>51</v>
+      </c>
       <c r="F7" s="13" t="s">
         <v>48</v>
       </c>
@@ -2252,13 +2263,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>47</v>
@@ -2277,13 +2288,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>47</v>
@@ -2302,13 +2313,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>47</v>
@@ -2325,91 +2336,121 @@
       </c>
       <c r="I10" s="16"/>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="B12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="E12" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="B13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="17"/>
+      <c r="B14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
+  <mergeCells count="5">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:D13 F4:H13">
+  <conditionalFormatting sqref="B5:D14 F5:H14">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -2421,7 +2462,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B4:D13 F4:H13" xr:uid="{FB37DCCE-CA2A-4DD7-B48E-169B1B1B1FCF}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B5:D14 F5:H14" xr:uid="{FB37DCCE-CA2A-4DD7-B48E-169B1B1B1FCF}">
       <formula1>"Not Tested, Failed, Passed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Implemented "Add VI or CTL to lvproj, lvlib, or lvclass.vi". This implements a new, better, more consistent way of inserting the newly created VI into a lvproj, lvlib, lvclass (including inserting into a virtual folder inside these project items).
</commit_message>
<xml_diff>
--- a/src/Design Documents/Design Spreadsheet.xlsx
+++ b/src/Design Documents/Design Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C708B880-1400-45E4-860E-E1D8519C1391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20B6598-5653-48BA-9561-8C9AA63C03C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Spreadsheet" sheetId="1" r:id="rId1"/>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="F14" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF71B33-42AD-4C32-A9F4-2F19848A426B}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Built LLB version 1.3.0.5 and successfully tested the VI and CTL creation functionality in initial states 9, 10, 11
</commit_message>
<xml_diff>
--- a/src/Design Documents/Design Spreadsheet.xlsx
+++ b/src/Design Documents/Design Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20B6598-5653-48BA-9561-8C9AA63C03C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B562FECA-07C2-47EC-9CBA-2200F6ED16FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="577" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Spreadsheet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="84">
   <si>
     <t>Design Spreadsheet</t>
   </si>
@@ -288,12 +288,25 @@
   <si>
     <t>Error 56002 occurs here too, just like in IS10. The VI or CTL is correctly inserted into the virtual folder.</t>
   </si>
+  <si>
+    <t>Assumed Passed</t>
+  </si>
+  <si>
+    <t>Test Date: 15 Dec 2022
+LLB Version: 1.3.0.5</t>
+  </si>
+  <si>
+    <t>The creation behaviour in Initial States 9, 10, 11 now passed.</t>
+  </si>
+  <si>
+    <t>Assumed Passed = Not tested, but relevant source code not modified. Therefore expected to continue passing.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +345,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -353,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -519,11 +539,144 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -562,22 +715,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -607,74 +796,239 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -1217,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:N6"/>
+    <sheetView topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,21 +1587,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1267,89 +1621,89 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
       <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="36"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="18"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="29" t="s">
+      <c r="I5" s="39"/>
+      <c r="J5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="27"/>
-      <c r="L5" s="30" t="s">
+      <c r="K5" s="39"/>
+      <c r="L5" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="27"/>
-      <c r="N5" s="29" t="s">
+      <c r="M5" s="39"/>
+      <c r="N5" s="31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
@@ -1368,28 +1722,28 @@
       <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="29"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="35" t="s">
+      <c r="A7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>50</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="16" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -1410,30 +1764,30 @@
       <c r="M7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="34" t="s">
+      <c r="N7" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="38" t="s">
+      <c r="A8" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H8" s="9" t="s">
@@ -1454,30 +1808,30 @@
       <c r="M8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="35" t="s">
+      <c r="A9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="34"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1496,30 +1850,30 @@
       <c r="M9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="N9" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="35" t="s">
+      <c r="A10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="16" t="s">
         <v>36</v>
       </c>
       <c r="H10" s="8" t="s">
@@ -1540,30 +1894,30 @@
       <c r="M10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="34" t="s">
+      <c r="N10" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="35" t="s">
+      <c r="A11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>53</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="16" t="s">
         <v>37</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -1584,30 +1938,30 @@
       <c r="M11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="34" t="s">
+      <c r="N11" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="38" t="s">
+      <c r="A12" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -1628,30 +1982,30 @@
       <c r="M12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="37" t="s">
+      <c r="N12" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="35" t="s">
+      <c r="A13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>54</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="34"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1670,30 +2024,30 @@
       <c r="M13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N13" s="34" t="s">
+      <c r="N13" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="35" t="s">
+      <c r="A14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>55</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="34"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1712,30 +2066,30 @@
       <c r="M14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="34" t="s">
+      <c r="N14" s="16" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="35" t="s">
+      <c r="A15" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>38</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="34"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1754,30 +2108,30 @@
       <c r="M15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N15" s="34" t="s">
+      <c r="N15" s="16" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="35" t="s">
+      <c r="A16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="34"/>
+      <c r="G16" s="16"/>
       <c r="H16" s="8" t="s">
         <v>14</v>
       </c>
@@ -1796,30 +2150,30 @@
       <c r="M16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N16" s="34" t="s">
+      <c r="N16" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="35" t="s">
+      <c r="A17" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="34"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="8" t="s">
         <v>14</v>
       </c>
@@ -1838,30 +2192,30 @@
       <c r="M17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="34" t="s">
+      <c r="N17" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="150" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="35" t="s">
+      <c r="A18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="34"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="8" t="s">
         <v>14</v>
       </c>
@@ -1880,30 +2234,30 @@
       <c r="M18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="38" t="s">
+      <c r="A19" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>62</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H19" s="9" t="s">
@@ -1924,30 +2278,30 @@
       <c r="M19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N19" s="37" t="s">
+      <c r="N19" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="38" t="s">
+      <c r="A20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>62</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H20" s="9" t="s">
@@ -1968,30 +2322,30 @@
       <c r="M20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="37" t="s">
+      <c r="N20" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="38" t="s">
+      <c r="A21" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>62</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H21" s="9" t="s">
@@ -2012,30 +2366,30 @@
       <c r="M21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="37" t="s">
+      <c r="N21" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="38" t="s">
+      <c r="A22" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>62</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="19" t="s">
         <v>63</v>
       </c>
       <c r="H22" s="9" t="s">
@@ -2056,7 +2410,7 @@
       <c r="M22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N22" s="37" t="s">
+      <c r="N22" s="19" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2086,10 +2440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF71B33-42AD-4C32-A9F4-2F19848A426B}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,18 +2454,18 @@
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:15" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
@@ -2120,17 +2474,17 @@
       <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
@@ -2139,51 +2493,51 @@
       <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="47"/>
     </row>
     <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="48" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="49" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -2195,7 +2549,7 @@
       <c r="D5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="13" t="s">
         <v>48</v>
       </c>
@@ -2205,10 +2559,10 @@
       <c r="H5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="50"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -2220,7 +2574,7 @@
       <c r="D6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>51</v>
       </c>
       <c r="F6" s="13" t="s">
@@ -2232,10 +2586,10 @@
       <c r="H6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="16"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="49" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -2247,7 +2601,7 @@
       <c r="D7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>51</v>
       </c>
       <c r="F7" s="13" t="s">
@@ -2259,10 +2613,10 @@
       <c r="H7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="50"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="49" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -2274,7 +2628,7 @@
       <c r="D8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="13" t="s">
         <v>48</v>
       </c>
@@ -2284,10 +2638,10 @@
       <c r="H8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="I8" s="50"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="49" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -2299,7 +2653,7 @@
       <c r="D9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="13" t="s">
         <v>48</v>
       </c>
@@ -2309,10 +2663,10 @@
       <c r="H9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="16"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="49" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -2324,7 +2678,7 @@
       <c r="D10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="13" t="s">
         <v>48</v>
       </c>
@@ -2334,10 +2688,10 @@
       <c r="H10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -2349,7 +2703,7 @@
       <c r="D11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="13" t="s">
         <v>48</v>
       </c>
@@ -2359,10 +2713,10 @@
       <c r="H11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="50"/>
     </row>
     <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="49" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -2374,7 +2728,7 @@
       <c r="D12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>76</v>
       </c>
       <c r="F12" s="13" t="s">
@@ -2386,10 +2740,10 @@
       <c r="H12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="16"/>
+      <c r="I12" s="50"/>
     </row>
     <row r="13" spans="1:15" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="49" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -2401,7 +2755,7 @@
       <c r="D13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>78</v>
       </c>
       <c r="F13" s="13" t="s">
@@ -2413,37 +2767,352 @@
       <c r="H13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="16"/>
-    </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="I13" s="50"/>
+    </row>
+    <row r="14" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="18" t="s">
+      <c r="B14" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" s="17"/>
+      <c r="F14" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="55"/>
+    </row>
+    <row r="15" spans="1:15" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="47"/>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="46"/>
+      <c r="B17" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="50"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="50"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="50"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="50"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="50"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="50"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="50"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="50"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="50"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="54"/>
+      <c r="F27" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="A1:I1"/>
@@ -2451,19 +3120,36 @@
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:D14 F5:H14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"Assumed Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:D27 F18:H27">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"Assumed Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B5:D14 F5:H14" xr:uid="{FB37DCCE-CA2A-4DD7-B48E-169B1B1B1FCF}">
-      <formula1>"Not Tested, Failed, Passed"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B5:D14 F5:H14 B18:D27 F18:H27" xr:uid="{FB37DCCE-CA2A-4DD7-B48E-169B1B1B1FCF}">
+      <formula1>"Not Tested, Failed, Assumed Passed, Passed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>